<commit_message>
execution time issue fixed
</commit_message>
<xml_diff>
--- a/Results/first_third/first_third_apriori_top_category_combinations.xlsx
+++ b/Results/first_third/first_third_apriori_top_category_combinations.xlsx
@@ -477,37 +477,37 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>964</v>
+        <v>936</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Storage &amp; Organization</t>
+          <t>Fashion &amp; Accessories</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Storage &amp; Organization</t>
+          <t>Fashion &amp; Accessories</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>522</v>
+        <v>508</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Fashion &amp; Accessories</t>
+          <t>Storage &amp; Organization</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Fashion &amp; Accessories</t>
+          <t>Storage &amp; Organization</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>508</v>
+        <v>490</v>
       </c>
     </row>
     <row r="6">
@@ -522,37 +522,37 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>410</v>
+        <v>400</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>Storage &amp; Organization</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>Kids &amp; Toys</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Storage &amp; Organization</t>
-        </is>
-      </c>
       <c r="C7" t="n">
-        <v>182</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>Kids &amp; Toys</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>Storage &amp; Organization</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Kids &amp; Toys</t>
-        </is>
-      </c>
       <c r="C8" t="n">
-        <v>182</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9">
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10">
@@ -582,22 +582,22 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Kitchen &amp; Dining</t>
+          <t>Kids &amp; Toys</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Storage &amp; Organization</t>
+          <t>Kids &amp; Toys</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed confidence and number of recommendations are included
</commit_message>
<xml_diff>
--- a/Results/first_third/first_third_apriori_top_category_combinations.xlsx
+++ b/Results/first_third/first_third_apriori_top_category_combinations.xlsx
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>936</v>
+        <v>466</v>
       </c>
     </row>
     <row r="4">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>508</v>
+        <v>396</v>
       </c>
     </row>
     <row r="5">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>490</v>
+        <v>297</v>
       </c>
     </row>
     <row r="6">
@@ -522,22 +522,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>400</v>
+        <v>228</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>Kids &amp; Toys</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>Storage &amp; Organization</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Kids &amp; Toys</t>
-        </is>
-      </c>
       <c r="C7" t="n">
-        <v>158</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8">
@@ -548,56 +548,56 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Storage &amp; Organization</t>
+          <t>Kids &amp; Toys</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>158</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>Fashion &amp; Accessories</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>Storage &amp; Organization</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Fashion &amp; Accessories</t>
-        </is>
-      </c>
       <c r="C9" t="n">
-        <v>150</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>Storage &amp; Organization</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>Fashion &amp; Accessories</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Storage &amp; Organization</t>
-        </is>
-      </c>
       <c r="C10" t="n">
-        <v>150</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>Storage &amp; Organization</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
           <t>Kids &amp; Toys</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Kids &amp; Toys</t>
-        </is>
-      </c>
       <c r="C11" t="n">
-        <v>120</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>